<commit_message>
Updated Mocap Planning Sheet
</commit_message>
<xml_diff>
--- a/Mocap Planning Sheet.xlsx
+++ b/Mocap Planning Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucreative-my.sharepoint.com/personal/u0007596_ucreative_ac_uk/Documents/01 Teaching 2025/FGCT5004 Motion Capture Technologies/Session02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucreative-my.sharepoint.com/personal/2311323_students_ucreative_ac_uk/Documents/Year 2 Animation/Motion Capture Elective/Year-2-MoCap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="379" documentId="8_{6DC7063A-DFB2-4A7F-96B9-493E01E1A7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0A25FFE-7D99-413B-AC9C-DF25C58FF1D2}"/>
+  <xr:revisionPtr revIDLastSave="408" documentId="8_{6DC7063A-DFB2-4A7F-96B9-493E01E1A7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7392D3B-8164-4CFD-A850-21213630A0B8}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="705" windowWidth="22335" windowHeight="12870" activeTab="1" xr2:uid="{20970AFA-7076-4E74-BB00-A72DD054B85C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{20970AFA-7076-4E74-BB00-A72DD054B85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>Props</t>
   </si>
@@ -134,9 +134,6 @@
   </si>
   <si>
     <t>Props List</t>
-  </si>
-  <si>
-    <t>ie Flash Light</t>
   </si>
   <si>
     <t>Y</t>
@@ -155,12 +152,6 @@
 (Male/Female)</t>
   </si>
   <si>
-    <t>i.e. Chun-Li</t>
-  </si>
-  <si>
-    <t>i.e.Lucy Brown</t>
-  </si>
-  <si>
     <t>To be motion captured (Y/N)</t>
   </si>
   <si>
@@ -171,6 +162,45 @@
   </si>
   <si>
     <t xml:space="preserve">*You will need to amend the estimated time required for each shot depending on what you are shooting and the complexity of the shot. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santa </t>
+  </si>
+  <si>
+    <t>Daniel Lock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miltary Solider </t>
+  </si>
+  <si>
+    <t>Santa Sack (Rubbish Bag)</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Presents (Boxes)</t>
+  </si>
+  <si>
+    <t>Markers (General loctions)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toys </t>
+  </si>
+  <si>
+    <t>Cookies</t>
+  </si>
+  <si>
+    <t>Chimney (Chairs/Mat)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bed (Mats) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gun </t>
   </si>
 </sst>
 </file>
@@ -660,13 +690,13 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
@@ -683,61 +713,120 @@
         <v>30</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C2" s="20">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="20"/>
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="20">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>37</v>
+      </c>
       <c r="C4" s="20"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
       <c r="C5" s="20"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
       <c r="C6" s="20"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
       <c r="C7" s="20"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
       <c r="C8" s="20"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
       <c r="C9" s="20"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
       <c r="C10" s="20"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>40</v>
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -750,7 +839,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -868,7 +957,7 @@
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -930,7 +1019,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>0</v>
@@ -939,7 +1028,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1175,7 +1264,7 @@
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
@@ -1297,7 +1386,7 @@
     </row>
     <row r="22" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J22" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Mocap Planning Sheet
All Categories Completed
</commit_message>
<xml_diff>
--- a/Mocap Planning Sheet.xlsx
+++ b/Mocap Planning Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucreative-my.sharepoint.com/personal/2311323_students_ucreative_ac_uk/Documents/Year 2 Animation/Motion Capture Elective/Year-2-MoCap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="484" documentId="8_{6DC7063A-DFB2-4A7F-96B9-493E01E1A7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2392FBB4-71EB-45C1-BC62-5A290C1194E9}"/>
+  <xr:revisionPtr revIDLastSave="541" documentId="8_{6DC7063A-DFB2-4A7F-96B9-493E01E1A7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A2B1598-71C3-4A45-9249-1987E135D1BD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{20970AFA-7076-4E74-BB00-A72DD054B85C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{20970AFA-7076-4E74-BB00-A72DD054B85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="84">
   <si>
     <t>Props</t>
   </si>
@@ -252,13 +252,52 @@
   </si>
   <si>
     <t xml:space="preserve">Drugged </t>
+  </si>
+  <si>
+    <t>Santa wobbles towards the tree and reaches for his sack to place presents. Santa kneels on one knee to reach under the tree and starts placing presents from inside the sack to under the tree.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santa Sack, Gun, Markers, Presents </t>
+  </si>
+  <si>
+    <t>Christmas Tree</t>
+  </si>
+  <si>
+    <t>Santa will keep his hands stuck to his sides as if he is trapped in a wreath. Military soldiers will approach him holding weapons after santa has been trapped. Santa will then fall to his knees or fall over due to the drugged cookies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trap Santa </t>
+  </si>
+  <si>
+    <t>Santa Sack, Gun, Markers, Mat</t>
+  </si>
+  <si>
+    <t>Santa will wake up in the cell from on the floor and then walks up to the bars and grips onto them and shakes.</t>
+  </si>
+  <si>
+    <t>Area 51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Markers, Bottels, Chairs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alien </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extras/Reshoots if needed </t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Alien</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +324,12 @@
       <sz val="11"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -349,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -410,6 +455,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,22 +794,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34A0C65F-A89E-4381-8657-7A4243518DB3}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
@@ -780,7 +826,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -797,7 +843,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -811,82 +857,95 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="20">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="20"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" s="20"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="20"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" s="20"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="20"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>44</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="20"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="20"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="20"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>28</v>
       </c>
     </row>
@@ -900,21 +959,21 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="6" width="8.7109375" style="1"/>
-    <col min="7" max="8" width="15.85546875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="35.109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="8.6640625" style="1"/>
+    <col min="7" max="8" width="15.88671875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="42.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
         <v>15</v>
       </c>
@@ -931,7 +990,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
@@ -947,7 +1006,7 @@
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -969,7 +1028,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -982,16 +1041,16 @@
       </c>
       <c r="D4" s="4">
         <f>IF(B3=0,"00:00",G4+(B3-1)*H4)</f>
-        <v>1.2500000000000001E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="G4" s="4">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="H4" s="4">
-        <v>5.5555555555555558E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -1000,7 +1059,7 @@
       </c>
       <c r="C5" s="4">
         <f t="shared" si="0"/>
-        <v>0.47083333333333338</v>
+        <v>0.47222222222222227</v>
       </c>
       <c r="D5" s="4">
         <f>IF(B5=0,"00:00",G5+(B5-1)*H5)</f>
@@ -1010,19 +1069,19 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="H5" s="4">
-        <v>4.8611111111111112E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" si="0"/>
-        <v>0.4777777777777778</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="13" t="s">
         <v>34</v>
       </c>
@@ -1038,27 +1097,27 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="7.42578125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" style="11" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="11" customWidth="1"/>
-    <col min="9" max="10" width="12.28515625" style="11" customWidth="1"/>
-    <col min="11" max="11" width="36.5703125" style="11" customWidth="1"/>
-    <col min="12" max="12" width="159.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.140625" style="11" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="11"/>
-    <col min="15" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="2" width="7.44140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" style="11" customWidth="1"/>
+    <col min="9" max="10" width="12.33203125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="36.5546875" style="11" customWidth="1"/>
+    <col min="12" max="12" width="205.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.109375" style="11" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" style="11"/>
+    <col min="15" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="42.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1099,7 +1158,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -1131,7 +1190,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -1164,7 +1223,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -1200,7 +1259,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -1233,7 +1292,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A6" s="11">
         <v>3</v>
       </c>
@@ -1269,7 +1328,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="11">
         <v>4</v>
       </c>
@@ -1305,7 +1364,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15" t="s">
@@ -1327,7 +1386,7 @@
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
     </row>
-    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15" t="s">
@@ -1349,7 +1408,7 @@
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>4</v>
       </c>
@@ -1385,52 +1444,118 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>5</v>
       </c>
       <c r="B11" s="11">
         <v>1</v>
       </c>
+      <c r="C11" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="11">
+        <v>3</v>
+      </c>
       <c r="I11" s="19">
         <f t="shared" si="0"/>
         <v>0.61111111111111094</v>
       </c>
       <c r="J11" s="14">
-        <v>6.9444444444444441E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B12" s="11">
+        <v>2</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="11">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="11">
+        <v>2</v>
+      </c>
+      <c r="I12" s="19">
+        <f t="shared" si="0"/>
+        <v>0.62152777777777757</v>
+      </c>
+      <c r="J12" s="14">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>6</v>
+      </c>
+      <c r="B13" s="11">
+        <v>1</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="11">
         <v>3</v>
       </c>
-      <c r="I12" s="19">
-        <f t="shared" si="0"/>
-        <v>0.61805555555555536</v>
-      </c>
-      <c r="J12" s="14">
-        <v>6.9444444444444441E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
-        <v>2</v>
-      </c>
-      <c r="B13" s="11">
+      <c r="E13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="11">
         <v>4</v>
       </c>
       <c r="I13" s="19">
         <f t="shared" si="0"/>
-        <v>0.62499999999999978</v>
+        <v>0.6319444444444442</v>
       </c>
       <c r="J13" s="14">
-        <v>6.9444444444444441E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>2</v>
       </c>
@@ -1439,13 +1564,13 @@
       </c>
       <c r="I14" s="19">
         <f t="shared" si="0"/>
-        <v>0.6319444444444442</v>
+        <v>0.64236111111111083</v>
       </c>
       <c r="J14" s="14">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="16" t="s">
@@ -1458,7 +1583,7 @@
       <c r="H15" s="15"/>
       <c r="I15" s="19">
         <f t="shared" si="0"/>
-        <v>0.63888888888888862</v>
+        <v>0.64930555555555525</v>
       </c>
       <c r="J15" s="16">
         <v>6.9444444444444441E-3</v>
@@ -1467,67 +1592,70 @@
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <v>2</v>
-      </c>
-      <c r="B16" s="11">
-        <v>5</v>
+    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="I16" s="19">
         <f t="shared" si="0"/>
-        <v>0.64583333333333304</v>
+        <v>0.65624999999999967</v>
       </c>
       <c r="J16" s="14">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
-        <v>2</v>
-      </c>
-      <c r="B17" s="11">
-        <v>6</v>
+    <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="I17" s="19">
         <f t="shared" si="0"/>
-        <v>0.65277777777777746</v>
+        <v>0.66319444444444409</v>
       </c>
       <c r="J17" s="14">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
-        <v>2</v>
-      </c>
-      <c r="B18" s="11">
-        <v>7</v>
+    <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="I18" s="19">
         <f t="shared" si="0"/>
-        <v>0.65972222222222188</v>
+        <v>0.67013888888888851</v>
       </c>
       <c r="J18" s="14">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
-        <v>2</v>
-      </c>
-      <c r="B19" s="11">
-        <v>8</v>
+    <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="I19" s="19">
         <f t="shared" si="0"/>
-        <v>0.6666666666666663</v>
+        <v>0.67708333333333293</v>
       </c>
       <c r="J19" s="14">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15" t="s">
@@ -1540,7 +1668,7 @@
       <c r="H20" s="15"/>
       <c r="I20" s="19">
         <f t="shared" si="0"/>
-        <v>0.67361111111111072</v>
+        <v>0.68402777777777735</v>
       </c>
       <c r="J20" s="16">
         <v>3.125E-2</v>
@@ -1549,7 +1677,7 @@
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
     </row>
-    <row r="21" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15" t="s">
@@ -1562,14 +1690,14 @@
       <c r="H21" s="15"/>
       <c r="I21" s="19">
         <f t="shared" si="0"/>
-        <v>0.70486111111111072</v>
+        <v>0.71527777777777735</v>
       </c>
       <c r="J21" s="16"/>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
     </row>
-    <row r="22" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J22" s="13" t="s">
         <v>36</v>
       </c>

</xml_diff>